<commit_message>
Misc updates and prefabs
Adding some prefabs and updating some settings
</commit_message>
<xml_diff>
--- a/Documentation/Design Documents/Design Scratch.xlsx
+++ b/Documentation/Design Documents/Design Scratch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Storage\Git\Project-SpellNote_Public\Documentation\Design Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155B53AF-6ABA-4B91-A152-932F23A91C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD20E3B-5070-46D8-A8DF-D4615FC4F282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Use music theory terms to inspire mechanics?</t>
   </si>
@@ -236,6 +236,18 @@
   </si>
   <si>
     <t>b/#</t>
+  </si>
+  <si>
+    <t>##/x</t>
+  </si>
+  <si>
+    <t>bb/x</t>
+  </si>
+  <si>
+    <t>x/##</t>
+  </si>
+  <si>
+    <t>x/bb</t>
   </si>
 </sst>
 </file>
@@ -553,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R56"/>
+  <dimension ref="A2:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="Q26" sqref="Q26:T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,22 +626,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -643,7 +655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -662,11 +674,8 @@
       <c r="I23" t="s">
         <v>40</v>
       </c>
-      <c r="R23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -679,21 +688,22 @@
       <c r="F24" t="s">
         <v>44</v>
       </c>
-      <c r="R24" t="s">
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>70</v>
+      </c>
+      <c r="R26" t="s">
+        <v>71</v>
+      </c>
+      <c r="S26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R26" t="s">
+      <c r="T26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>30</v>
       </c>
@@ -706,8 +716,20 @@
       <c r="F27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>72</v>
+      </c>
+      <c r="R27" t="s">
+        <v>73</v>
+      </c>
+      <c r="S27" t="s">
+        <v>68</v>
+      </c>
+      <c r="T27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>32</v>
       </c>
@@ -715,17 +737,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>47</v>
       </c>

</xml_diff>